<commit_message>
update test cases template
</commit_message>
<xml_diff>
--- a/testcases/test-cases-template.xlsx
+++ b/testcases/test-cases-template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Project Name:</t>
   </si>
@@ -343,9 +343,6 @@
       </rPr>
       <t>(Segun el dominio de: la app, la logica de negocio)</t>
     </r>
-  </si>
-  <si>
-    <t>https://www.javatpoint.com/structural-testing</t>
   </si>
   <si>
     <r>
@@ -782,7 +779,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -873,6 +870,36 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -896,33 +923,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1266,68 +1266,68 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="33">
         <v>1</v>
       </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="32"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="39"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="44">
         <v>44567</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
@@ -1340,45 +1340,45 @@
       <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="32"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="37">
         <v>44567</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="39"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
@@ -1393,10 +1393,10 @@
       <c r="A10" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="44"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
@@ -1406,10 +1406,10 @@
       <c r="A11" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
@@ -1419,10 +1419,10 @@
       <c r="A12" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="44"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
@@ -1432,10 +1432,10 @@
       <c r="A13" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="44"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
@@ -1443,12 +1443,12 @@
     </row>
     <row r="14" spans="1:7" ht="24">
       <c r="A14" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="44"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
@@ -1456,12 +1456,12 @@
     </row>
     <row r="15" spans="1:7" ht="24">
       <c r="A15" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="45"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
@@ -1471,10 +1471,10 @@
       <c r="A16" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="45"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
@@ -1482,12 +1482,12 @@
     </row>
     <row r="17" spans="1:7" ht="24">
       <c r="A17" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="45"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
@@ -1497,10 +1497,10 @@
       <c r="A18" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="45"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="8"/>
@@ -1510,10 +1510,10 @@
       <c r="A19" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="45"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="8"/>
@@ -1521,12 +1521,12 @@
     </row>
     <row r="20" spans="1:7" ht="24">
       <c r="A20" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="45"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="8"/>
@@ -1536,10 +1536,10 @@
       <c r="A21" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="45"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="8"/>
@@ -1547,12 +1547,12 @@
     </row>
     <row r="22" spans="1:7" ht="24">
       <c r="A22" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
@@ -1562,10 +1562,10 @@
       <c r="A23" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="45"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
       <c r="F23" s="8"/>
@@ -1573,25 +1573,23 @@
     </row>
     <row r="24" spans="1:7" ht="24">
       <c r="A24" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="27" t="s">
-        <v>69</v>
-      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="7"/>
       <c r="F24" s="8"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="24">
       <c r="A25" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="27"/>
@@ -1601,12 +1599,12 @@
     </row>
     <row r="26" spans="1:7" ht="24">
       <c r="A26" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="45"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="27"/>
       <c r="E26" s="7"/>
       <c r="F26" s="8"/>
@@ -1625,10 +1623,10 @@
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="44"/>
+      <c r="C28" s="36"/>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
@@ -1638,10 +1636,10 @@
       <c r="A29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="44"/>
+      <c r="C29" s="36"/>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
@@ -1651,10 +1649,10 @@
       <c r="A30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="36"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
       <c r="F30" s="8"/>
@@ -1664,10 +1662,10 @@
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="39"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -1677,8 +1675,8 @@
       <c r="A32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -1845,6 +1843,28 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A2:G3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B22:C22"/>
@@ -1855,28 +1875,6 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="A2:G3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="F40">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="fail">
@@ -1902,10 +1900,7 @@
       <formula>NOT(ISERROR(SEARCH("pass",F41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="D24" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>